<commit_message>
include C Ack and Univ opt
</commit_message>
<xml_diff>
--- a/SID-mapping-bis.xlsx
+++ b/SID-mapping-bis.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurent/Library/CloudStorage/OneDrive-Personnel/Documents/xlapak/schc-wg/YANG-DM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4733D08A-688C-7C41-A2CB-7E5C67081822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{95BB1D34-7A80-A246-BA94-D8595264FFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="900" windowWidth="36000" windowHeight="20480" xr2:uid="{79CBBA98-45D0-AB4B-8F46-38D859212AB5}"/>
   </bookViews>
   <sheets>
-    <sheet name="SID Allocation" sheetId="1" r:id="rId1"/>
+    <sheet name="SID-mapping-bis" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil1" sheetId="3" r:id="rId2"/>
     <sheet name="excluded SID" sheetId="2" r:id="rId3"/>
   </sheets>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="180">
   <si>
     <t>module</t>
   </si>
@@ -514,15 +514,6 @@
     <t>bitmap-compound-ack</t>
   </si>
   <si>
-    <t>/ietf-schc:schc/rule/ietf-schc-compound-ack:bitmap-format</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data </t>
-  </si>
-  <si>
-    <t>/ietf-schc:schc/rule/ietf-schc-compound-ack:last-bitmap-compression</t>
-  </si>
-  <si>
     <t xml:space="preserve"> space-id-base-type</t>
   </si>
   <si>
@@ -581,6 +572,12 @@
   </si>
   <si>
     <t>/ietf-schc:schc/rule/universal-option-entry/target-value/value</t>
+  </si>
+  <si>
+    <t>/ietf-schc:schc/rule/bitmap-format</t>
+  </si>
+  <si>
+    <t>/ietf-schc:schc/rule/last-bitmap-compression</t>
   </si>
 </sst>
 </file>
@@ -988,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CAE7973-9DF4-B240-B0AB-F84379B61AEA}">
   <dimension ref="A1:E400"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54:B70"/>
+    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
+      <selection activeCell="C246" sqref="C246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1383,10 +1380,10 @@
         <v>3</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -1398,10 +1395,10 @@
         <v>3</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -1413,10 +1410,10 @@
         <v>3</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -1428,10 +1425,10 @@
         <v>3</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -1443,10 +1440,10 @@
         <v>3</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -1458,10 +1455,10 @@
         <v>3</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -1473,10 +1470,10 @@
         <v>3</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -1488,10 +1485,10 @@
         <v>3</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -1503,10 +1500,10 @@
         <v>3</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -1518,10 +1515,10 @@
         <v>3</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -1533,10 +1530,10 @@
         <v>3</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -1548,10 +1545,10 @@
         <v>3</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -1563,10 +1560,10 @@
         <v>3</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -1578,10 +1575,10 @@
         <v>3</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -1593,10 +1590,10 @@
         <v>3</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -1608,10 +1605,10 @@
         <v>3</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -1623,10 +1620,10 @@
         <v>3</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -2274,7 +2271,7 @@
         <v>3</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="D115" s="3" t="s">
         <v>156</v>
@@ -2286,10 +2283,10 @@
         <v>2665</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>159</v>
+        <v>3</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>160</v>
+        <v>179</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>156</v>
@@ -3045,13 +3042,13 @@
         <v>2790</v>
       </c>
       <c r="B241" s="4" t="s">
-        <v>152</v>
+        <v>49</v>
       </c>
       <c r="C241" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D241" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
@@ -4721,7 +4718,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1">
-        <f>'SID Allocation'!A327+1</f>
+        <f>'SID-mapping-bis'!A327+1</f>
         <v>2877</v>
       </c>
       <c r="B1" t="s">
@@ -4868,7 +4865,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
-        <f>'SID Allocation'!A343+1</f>
+        <f>'SID-mapping-bis'!A343+1</f>
         <v>2893</v>
       </c>
       <c r="B14" t="s">
@@ -5113,10 +5110,10 @@
         <v>49</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>